<commit_message>
updated the way values are merge to be more likely to get large groups and to always find the all group
</commit_message>
<xml_diff>
--- a/static/marchMadness/marchMadnessTesting.xlsx
+++ b/static/marchMadness/marchMadnessTesting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/marchMadness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9D9301-36EA-4781-9417-AEA7BA861B59}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{59FA6CC9-D02C-444C-8C9B-7D565C1F61C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -573,11 +573,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909BC3E6-1313-4909-83D8-6D1A2BDCBA9C}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J28" workbookViewId="0">
-      <selection activeCell="U50" sqref="U50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="6" max="6" width="14.26171875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -671,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K2), $K$16:$P$16)</f>
+        <f t="shared" ref="R2:R14" si="0">SUMPRODUCT(_xlfn.ANCHORARRAY(K2), $K$16:$P$16)</f>
         <v>980</v>
       </c>
       <c r="S2" s="2">
@@ -683,7 +686,7 @@
         <v>1003</v>
       </c>
       <c r="V2">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K2), $K$21:$P$21)</f>
+        <f t="shared" ref="V2:V14" si="1">SUMPRODUCT(_xlfn.ANCHORARRAY(K2), $K$21:$P$21)</f>
         <v>1660</v>
       </c>
       <c r="W2" s="2">
@@ -757,19 +760,19 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K3), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>820</v>
       </c>
       <c r="S3" s="2">
-        <f t="shared" ref="S3:S14" si="0">R3 / SUM($R$2:$R$14)</f>
+        <f t="shared" ref="S3:S14" si="2">R3 / SUM($R$2:$R$14)</f>
         <v>9.2446448703494929E-2</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T14" si="1">R3 + D3 + G3 * 10</f>
+        <f t="shared" ref="T3:T14" si="3">R3 + D3 + G3 * 10</f>
         <v>850</v>
       </c>
       <c r="V3">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K3), $K$21:$P$21)</f>
+        <f t="shared" si="1"/>
         <v>1410</v>
       </c>
       <c r="W3" s="2">
@@ -777,27 +780,27 @@
         <v>9.2156862745098045E-2</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X14" si="2">V3 + 2*D3 + G3 * 25</f>
+        <f t="shared" ref="X3:X14" si="4">V3 + 2*D3 + G3 * 25</f>
         <v>1475</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y14" si="3">_xlfn.RANK.AVG(X3, $X$2:$X$14)</f>
+        <f t="shared" ref="Y3:Y14" si="5">_xlfn.RANK.AVG(X3, $X$2:$X$14)</f>
         <v>2</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA14" si="4">SUMPRODUCT(_xlfn.ANCHORARRAY(K3), $R$16:$W$16)</f>
+        <f t="shared" ref="AA3:AA14" si="6">SUMPRODUCT(_xlfn.ANCHORARRAY(K3), $R$16:$W$16)</f>
         <v>760</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB14" si="5">AA3 / SUM($V$2:$V$14)</f>
+        <f t="shared" ref="AB3:AB14" si="7">AA3 / SUM($V$2:$V$14)</f>
         <v>4.9673202614379082E-2</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC14" si="6">AA3 + D3 + G3 * 10</f>
+        <f t="shared" ref="AC3:AC14" si="8">AA3 + D3 + G3 * 10</f>
         <v>790</v>
       </c>
       <c r="AD3">
-        <f t="shared" ref="AD3:AD14" si="7">_xlfn.RANK.AVG(AC3, $AC$2:$AC$14)</f>
+        <f t="shared" ref="AD3:AD14" si="9">_xlfn.RANK.AVG(AC3, $AC$2:$AC$14)</f>
         <v>2</v>
       </c>
     </row>
@@ -843,47 +846,47 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K4), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>770</v>
       </c>
       <c r="S4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.6809470124013535E-2</v>
       </c>
       <c r="T4">
+        <f t="shared" si="3"/>
+        <v>806</v>
+      </c>
+      <c r="V4">
         <f t="shared" si="1"/>
-        <v>806</v>
-      </c>
-      <c r="V4">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K4), $K$21:$P$21)</f>
         <v>1330</v>
       </c>
       <c r="W4" s="2">
-        <f t="shared" ref="W3:W14" si="8">V4 / SUM($V$2:$V$14)</f>
+        <f t="shared" ref="W4:W14" si="10">V4 / SUM($V$2:$V$14)</f>
         <v>8.6928104575163395E-2</v>
       </c>
       <c r="X4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1407</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>720</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.7058823529411764E-2</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>756</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -929,47 +932,47 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K5), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>780</v>
       </c>
       <c r="S5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.7936865839909811E-2</v>
       </c>
       <c r="T5">
+        <f t="shared" si="3"/>
+        <v>802</v>
+      </c>
+      <c r="V5">
         <f t="shared" si="1"/>
-        <v>802</v>
-      </c>
-      <c r="V5">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K5), $K$21:$P$21)</f>
         <v>1330</v>
       </c>
       <c r="W5" s="2">
+        <f t="shared" si="10"/>
+        <v>8.6928104575163395E-2</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="4"/>
+        <v>1374</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="6"/>
+        <v>750</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="7"/>
+        <v>4.9019607843137254E-2</v>
+      </c>
+      <c r="AC5">
         <f t="shared" si="8"/>
-        <v>8.6928104575163395E-2</v>
-      </c>
-      <c r="X5">
-        <f t="shared" si="2"/>
-        <v>1374</v>
-      </c>
-      <c r="Y5">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" si="4"/>
-        <v>750</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" si="5"/>
-        <v>4.9019607843137254E-2</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="6"/>
         <v>772</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1015,47 +1018,47 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K6), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>730</v>
       </c>
       <c r="S6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.2299887260428417E-2</v>
       </c>
       <c r="T6">
+        <f t="shared" si="3"/>
+        <v>756</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="1"/>
-        <v>756</v>
-      </c>
-      <c r="V6">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K6), $K$21:$P$21)</f>
         <v>1250</v>
       </c>
       <c r="W6" s="2">
+        <f t="shared" si="10"/>
+        <v>8.1699346405228759E-2</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="4"/>
+        <v>1312</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="6"/>
+        <v>680</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="7"/>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="AC6">
         <f t="shared" si="8"/>
-        <v>8.1699346405228759E-2</v>
-      </c>
-      <c r="X6">
-        <f t="shared" si="2"/>
-        <v>1312</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="4"/>
-        <v>680</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" si="5"/>
-        <v>4.4444444444444446E-2</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="6"/>
         <v>706</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
     </row>
@@ -1101,47 +1104,47 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K7), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="S7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.8917700112739575E-2</v>
       </c>
       <c r="T7">
+        <f t="shared" si="3"/>
+        <v>731</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="1"/>
-        <v>731</v>
-      </c>
-      <c r="V7">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K7), $K$21:$P$21)</f>
         <v>1210</v>
       </c>
       <c r="W7" s="2">
+        <f t="shared" si="10"/>
+        <v>7.9084967320261434E-2</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="4"/>
+        <v>1277</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="6"/>
+        <v>690</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="7"/>
+        <v>4.5098039215686274E-2</v>
+      </c>
+      <c r="AC7">
         <f t="shared" si="8"/>
-        <v>7.9084967320261434E-2</v>
-      </c>
-      <c r="X7">
-        <f t="shared" si="2"/>
-        <v>1277</v>
-      </c>
-      <c r="Y7">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="4"/>
-        <v>690</v>
-      </c>
-      <c r="AB7">
-        <f t="shared" si="5"/>
-        <v>4.5098039215686274E-2</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="6"/>
         <v>721</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -1187,47 +1190,47 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K8), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>620</v>
       </c>
       <c r="S8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.9898534385569339E-2</v>
       </c>
       <c r="T8">
+        <f t="shared" si="3"/>
+        <v>673</v>
+      </c>
+      <c r="V8">
         <f t="shared" si="1"/>
-        <v>673</v>
-      </c>
-      <c r="V8">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K8), $K$21:$P$21)</f>
         <v>1080</v>
       </c>
       <c r="W8" s="2">
+        <f t="shared" si="10"/>
+        <v>7.0588235294117646E-2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="4"/>
+        <v>1201</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="7"/>
+        <v>3.9215686274509803E-2</v>
+      </c>
+      <c r="AC8">
         <f t="shared" si="8"/>
-        <v>7.0588235294117646E-2</v>
-      </c>
-      <c r="X8">
-        <f t="shared" si="2"/>
-        <v>1201</v>
-      </c>
-      <c r="Y8">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="4"/>
-        <v>600</v>
-      </c>
-      <c r="AB8">
-        <f t="shared" si="5"/>
-        <v>3.9215686274509803E-2</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="6"/>
         <v>653</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
     </row>
@@ -1273,47 +1276,47 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K9), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>650</v>
       </c>
       <c r="S9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.3280721533258167E-2</v>
       </c>
       <c r="T9">
+        <f t="shared" si="3"/>
+        <v>667</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="1"/>
-        <v>667</v>
-      </c>
-      <c r="V9">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K9), $K$21:$P$21)</f>
         <v>1120</v>
       </c>
       <c r="W9" s="2">
+        <f t="shared" si="10"/>
+        <v>7.3202614379084971E-2</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="4"/>
+        <v>1154</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="6"/>
+        <v>640</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="7"/>
+        <v>4.1830065359477121E-2</v>
+      </c>
+      <c r="AC9">
         <f t="shared" si="8"/>
-        <v>7.3202614379084971E-2</v>
-      </c>
-      <c r="X9">
-        <f t="shared" si="2"/>
-        <v>1154</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="4"/>
-        <v>640</v>
-      </c>
-      <c r="AB9">
-        <f t="shared" si="5"/>
-        <v>4.1830065359477121E-2</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="6"/>
         <v>657</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
     </row>
@@ -1359,47 +1362,47 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K10), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>620</v>
       </c>
       <c r="S10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.9898534385569339E-2</v>
       </c>
       <c r="T10">
+        <f t="shared" si="3"/>
+        <v>667</v>
+      </c>
+      <c r="V10">
         <f t="shared" si="1"/>
-        <v>667</v>
-      </c>
-      <c r="V10">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K10), $K$21:$P$21)</f>
         <v>1080</v>
       </c>
       <c r="W10" s="2">
+        <f t="shared" si="10"/>
+        <v>7.0588235294117646E-2</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="4"/>
+        <v>1194</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="6"/>
+        <v>610</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="7"/>
+        <v>3.9869281045751631E-2</v>
+      </c>
+      <c r="AC10">
         <f t="shared" si="8"/>
-        <v>7.0588235294117646E-2</v>
-      </c>
-      <c r="X10">
-        <f t="shared" si="2"/>
-        <v>1194</v>
-      </c>
-      <c r="Y10">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="4"/>
-        <v>610</v>
-      </c>
-      <c r="AB10">
-        <f t="shared" si="5"/>
-        <v>3.9869281045751631E-2</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="6"/>
         <v>657</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
     </row>
@@ -1445,47 +1448,47 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K11), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="S11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.7643742953776773E-2</v>
       </c>
       <c r="T11">
+        <f t="shared" si="3"/>
+        <v>619</v>
+      </c>
+      <c r="V11">
         <f t="shared" si="1"/>
-        <v>619</v>
-      </c>
-      <c r="V11">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K11), $K$21:$P$21)</f>
         <v>1040</v>
       </c>
       <c r="W11" s="2">
+        <f t="shared" si="10"/>
+        <v>6.7973856209150321E-2</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="4"/>
+        <v>1083</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="6"/>
+        <v>580</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="7"/>
+        <v>3.7908496732026141E-2</v>
+      </c>
+      <c r="AC11">
         <f t="shared" si="8"/>
-        <v>6.7973856209150321E-2</v>
-      </c>
-      <c r="X11">
-        <f t="shared" si="2"/>
-        <v>1083</v>
-      </c>
-      <c r="Y11">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="4"/>
-        <v>580</v>
-      </c>
-      <c r="AB11">
-        <f t="shared" si="5"/>
-        <v>3.7908496732026141E-2</v>
-      </c>
-      <c r="AC11">
-        <f t="shared" si="6"/>
         <v>599</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
     </row>
@@ -1531,47 +1534,47 @@
         <v>0</v>
       </c>
       <c r="R12">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K12), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>560</v>
       </c>
       <c r="S12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.3134160090191654E-2</v>
       </c>
       <c r="T12">
+        <f t="shared" si="3"/>
+        <v>582</v>
+      </c>
+      <c r="V12">
         <f t="shared" si="1"/>
-        <v>582</v>
-      </c>
-      <c r="V12">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K12), $K$21:$P$21)</f>
         <v>970</v>
       </c>
       <c r="W12" s="2">
+        <f t="shared" si="10"/>
+        <v>6.3398692810457513E-2</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="4"/>
+        <v>1019</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="6"/>
+        <v>540</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="7"/>
+        <v>3.5294117647058823E-2</v>
+      </c>
+      <c r="AC12">
         <f t="shared" si="8"/>
-        <v>6.3398692810457513E-2</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="2"/>
-        <v>1019</v>
-      </c>
-      <c r="Y12">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="4"/>
-        <v>540</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="5"/>
-        <v>3.5294117647058823E-2</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="6"/>
         <v>562</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
     </row>
@@ -1617,47 +1620,47 @@
         <v>0</v>
       </c>
       <c r="R13">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K13), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>540</v>
       </c>
       <c r="S13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0879368658399095E-2</v>
       </c>
       <c r="T13">
+        <f t="shared" si="3"/>
+        <v>578</v>
+      </c>
+      <c r="V13">
         <f t="shared" si="1"/>
-        <v>578</v>
-      </c>
-      <c r="V13">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K13), $K$21:$P$21)</f>
         <v>940</v>
       </c>
       <c r="W13" s="2">
+        <f t="shared" si="10"/>
+        <v>6.1437908496732023E-2</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="4"/>
+        <v>1031</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="6"/>
+        <v>500</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="7"/>
+        <v>3.2679738562091505E-2</v>
+      </c>
+      <c r="AC13">
         <f t="shared" si="8"/>
-        <v>6.1437908496732023E-2</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="2"/>
-        <v>1031</v>
-      </c>
-      <c r="Y13">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="AA13">
-        <f t="shared" si="4"/>
-        <v>500</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="5"/>
-        <v>3.2679738562091505E-2</v>
-      </c>
-      <c r="AC13">
-        <f t="shared" si="6"/>
         <v>538</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
     </row>
@@ -1703,47 +1706,47 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K14), $K$16:$P$16)</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="S14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.6369785794813977E-2</v>
       </c>
       <c r="T14">
+        <f t="shared" si="3"/>
+        <v>537</v>
+      </c>
+      <c r="V14">
         <f t="shared" si="1"/>
-        <v>537</v>
-      </c>
-      <c r="V14">
-        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(K14), $K$21:$P$21)</f>
         <v>880</v>
       </c>
       <c r="W14" s="2">
+        <f t="shared" si="10"/>
+        <v>5.7516339869281043E-2</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="4"/>
+        <v>964</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="6"/>
+        <v>490</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="7"/>
+        <v>3.202614379084967E-2</v>
+      </c>
+      <c r="AC14">
         <f t="shared" si="8"/>
-        <v>5.7516339869281043E-2</v>
-      </c>
-      <c r="X14">
-        <f t="shared" si="2"/>
-        <v>964</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="4"/>
-        <v>490</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="5"/>
-        <v>3.202614379084967E-2</v>
-      </c>
-      <c r="AC14">
-        <f t="shared" si="6"/>
         <v>527</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
     </row>
@@ -1762,15 +1765,15 @@
         <v>30</v>
       </c>
       <c r="N16">
-        <f t="shared" ref="N16:P16" si="9">L16 + M16</f>
+        <f t="shared" ref="N16:P16" si="11">L16 + M16</f>
         <v>50</v>
       </c>
       <c r="O16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>80</v>
       </c>
       <c r="P16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>130</v>
       </c>
       <c r="R16">
@@ -1794,27 +1797,27 @@
     </row>
     <row r="17" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K17">
-        <f>K16 / $K$16</f>
+        <f t="shared" ref="K17:P17" si="12">K16 / $K$16</f>
         <v>1</v>
       </c>
       <c r="L17">
-        <f>L16 / $K$16</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="M17">
-        <f>M16 / $K$16</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="N17">
-        <f>N16 / $K$16</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="O17">
-        <f>O16 / $K$16</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P17">
-        <f>P16 / $K$16</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
     </row>
@@ -1874,37 +1877,37 @@
         <v>80</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="N21:P21" si="10">M21 + N21</f>
+        <f t="shared" ref="O21:P21" si="13">M21 + N21</f>
         <v>130</v>
       </c>
       <c r="P21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>210</v>
       </c>
     </row>
     <row r="22" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K22">
-        <f>K21 / $K$21</f>
+        <f t="shared" ref="K22:P22" si="14">K21 / $K$21</f>
         <v>1</v>
       </c>
       <c r="L22">
-        <f>L21 / $K$21</f>
+        <f t="shared" si="14"/>
         <v>1.5</v>
       </c>
       <c r="M22">
-        <f>M21 / $K$21</f>
+        <f t="shared" si="14"/>
         <v>2.5</v>
       </c>
       <c r="N22">
-        <f>N21 / $K$21</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="O22">
-        <f>O21 / $K$21</f>
+        <f t="shared" si="14"/>
         <v>6.5</v>
       </c>
       <c r="P22">
-        <f>P21 / $K$21</f>
+        <f t="shared" si="14"/>
         <v>10.5</v>
       </c>
     </row>
@@ -1954,23 +1957,23 @@
         <v>0.24489795918367346</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26:P26" si="11">L2 * L$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K2))</f>
+        <f t="shared" ref="L26:P26" si="15">L2 * L$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K2))</f>
         <v>0.22448979591836735</v>
       </c>
       <c r="M26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="N26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.10204081632653061</v>
       </c>
       <c r="O26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>8.1632653061224483E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.1326530612244898</v>
       </c>
       <c r="R26">
@@ -1982,469 +1985,469 @@
         <v>2.5694615195475778E-2</v>
       </c>
       <c r="T26">
-        <f t="shared" ref="S26:W26" si="12">M26 - M40</f>
+        <f t="shared" ref="T26:W26" si="16">M26 - M40</f>
         <v>3.4423407917383575E-3</v>
       </c>
       <c r="U26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>5.6552741578559107E-3</v>
       </c>
       <c r="V26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.3194000491762882E-3</v>
       </c>
       <c r="W26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>6.1470371281042713E-3</v>
       </c>
     </row>
     <row r="27" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K27">
-        <f t="shared" ref="K27:P27" si="13">K3 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K3))</f>
+        <f t="shared" ref="K27:P27" si="17">K3 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K3))</f>
         <v>0.3048780487804878</v>
       </c>
       <c r="L27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.1951219512195122</v>
       </c>
       <c r="M27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.21951219512195122</v>
       </c>
       <c r="N27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.18292682926829268</v>
       </c>
       <c r="O27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>9.7560975609756101E-2</v>
       </c>
       <c r="P27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R27">
-        <f t="shared" ref="R27:R38" si="14">K27 - K41</f>
+        <f t="shared" ref="R27:R38" si="18">K27 - K41</f>
         <v>-4.9731880297526398E-2</v>
       </c>
       <c r="S27">
-        <f t="shared" ref="S27:S38" si="15">L27 - L41</f>
+        <f t="shared" ref="S27:S38" si="19">L27 - L41</f>
         <v>2.4909185262065398E-2</v>
       </c>
       <c r="T27">
-        <f t="shared" ref="T27:T38" si="16">M27 - M41</f>
+        <f t="shared" ref="T27:T38" si="20">M27 - M41</f>
         <v>6.7462376751427078E-3</v>
       </c>
       <c r="U27">
-        <f t="shared" ref="U27:U38" si="17">N27 - N41</f>
+        <f t="shared" ref="U27:U38" si="21">N27 - N41</f>
         <v>1.2714063310845874E-2</v>
       </c>
       <c r="V27">
-        <f t="shared" ref="V27:V38" si="18">O27 - O41</f>
+        <f t="shared" ref="V27:V38" si="22">O27 - O41</f>
         <v>5.3623940494724187E-3</v>
       </c>
       <c r="W27">
-        <f t="shared" ref="W27:W38" si="19">P27 - P41</f>
+        <f t="shared" ref="W27:W38" si="23">P27 - P41</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K28">
-        <f t="shared" ref="K28:P28" si="20">K4 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K4))</f>
+        <f t="shared" ref="K28:P28" si="24">K4 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K4))</f>
         <v>0.35064935064935066</v>
       </c>
       <c r="L28">
+        <f t="shared" si="24"/>
+        <v>0.25974025974025972</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="24"/>
+        <v>0.15584415584415584</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="24"/>
+        <v>0.12987012987012986</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="24"/>
+        <v>0.1038961038961039</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="18"/>
+        <v>-5.5365686944634285E-2</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="19"/>
+        <v>3.4176349965823638E-2</v>
+      </c>
+      <c r="T28">
         <f t="shared" si="20"/>
-        <v>0.25974025974025972</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="20"/>
-        <v>0.15584415584415584</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="20"/>
-        <v>0.12987012987012986</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="20"/>
-        <v>0.1038961038961039</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="14"/>
-        <v>-5.5365686944634285E-2</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="15"/>
-        <v>3.4176349965823638E-2</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="16"/>
         <v>5.4682159945317887E-3</v>
       </c>
       <c r="U28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>9.5693779904306164E-3</v>
       </c>
       <c r="V28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>6.1517429938482693E-3</v>
       </c>
       <c r="W28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K29">
-        <f t="shared" ref="K29:P29" si="21">K5 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K5))</f>
+        <f t="shared" ref="K29:P29" si="25">K5 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K5))</f>
         <v>0.29487179487179488</v>
       </c>
       <c r="L29">
+        <f t="shared" si="25"/>
+        <v>0.28205128205128205</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="25"/>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="25"/>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="18"/>
+        <v>-5.099286678234044E-2</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="19"/>
+        <v>3.3930981299402363E-2</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="20"/>
+        <v>5.2053209947947043E-3</v>
+      </c>
+      <c r="U29">
         <f t="shared" si="21"/>
-        <v>0.28205128205128205</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="21"/>
-        <v>0.23076923076923078</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="21"/>
-        <v>0.19230769230769232</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="14"/>
-        <v>-5.099286678234044E-2</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="15"/>
-        <v>3.3930981299402363E-2</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="16"/>
-        <v>5.2053209947947043E-3</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="17"/>
         <v>1.1856564488143456E-2</v>
       </c>
       <c r="V29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K30">
-        <f t="shared" ref="K30:P30" si="22">K6 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K6))</f>
+        <f t="shared" ref="K30:P30" si="26">K6 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K6))</f>
         <v>0.30136986301369861</v>
       </c>
       <c r="L30">
+        <f t="shared" si="26"/>
+        <v>0.24657534246575341</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="26"/>
+        <v>0.20547945205479451</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="26"/>
+        <v>0.13698630136986301</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="26"/>
+        <v>0.1095890410958904</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="18"/>
+        <v>-5.0630136986301366E-2</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="19"/>
+        <v>3.0575342465753413E-2</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="20"/>
+        <v>5.479452054794498E-3</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="21"/>
+        <v>8.9863013698630034E-3</v>
+      </c>
+      <c r="V30">
         <f t="shared" si="22"/>
-        <v>0.24657534246575341</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="22"/>
-        <v>0.20547945205479451</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="22"/>
-        <v>0.13698630136986301</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="22"/>
-        <v>0.1095890410958904</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="14"/>
-        <v>-5.0630136986301366E-2</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="15"/>
-        <v>3.0575342465753413E-2</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="16"/>
-        <v>5.479452054794498E-3</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="17"/>
-        <v>8.9863013698630034E-3</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="18"/>
         <v>5.5890410958904096E-3</v>
       </c>
       <c r="W30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K31">
-        <f t="shared" ref="K31:P31" si="23">K7 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K7))</f>
+        <f t="shared" ref="K31:P31" si="27">K7 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K7))</f>
         <v>0.34285714285714286</v>
       </c>
       <c r="L31">
+        <f t="shared" si="27"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="27"/>
+        <v>0.3</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="27"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="18"/>
+        <v>-5.3837072018890209E-2</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="19"/>
+        <v>3.778040141676503E-2</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="20"/>
+        <v>1.0743801652892571E-2</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="21"/>
+        <v>5.3128689492325798E-3</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="W31">
         <f t="shared" si="23"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="23"/>
-        <v>0.3</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="23"/>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="14"/>
-        <v>-5.3837072018890209E-2</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="15"/>
-        <v>3.778040141676503E-2</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="16"/>
-        <v>1.0743801652892571E-2</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="17"/>
-        <v>5.3128689492325798E-3</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="W31">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K32">
-        <f t="shared" ref="K32:P32" si="24">K8 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K8))</f>
+        <f t="shared" ref="K32:P32" si="28">K8 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K8))</f>
         <v>0.40322580645161288</v>
       </c>
       <c r="L32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.29032258064516131</v>
       </c>
       <c r="M32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.14516129032258066</v>
       </c>
       <c r="N32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.16129032258064516</v>
       </c>
       <c r="O32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="R32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-5.9737156511350087E-2</v>
       </c>
       <c r="S32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4.032258064516131E-2</v>
       </c>
       <c r="T32">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>6.27240143369176E-3</v>
       </c>
       <c r="U32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.3142174432497017E-2</v>
       </c>
       <c r="V32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K33">
-        <f t="shared" ref="K33:P33" si="25">K9 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K9))</f>
+        <f t="shared" ref="K33:P33" si="29">K9 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K9))</f>
         <v>0.35384615384615387</v>
       </c>
       <c r="L33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.33846153846153848</v>
       </c>
       <c r="M33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="N33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="O33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-5.6868131868131833E-2</v>
       </c>
       <c r="S33">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4.381868131868133E-2</v>
       </c>
       <c r="T33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>7.5549450549450559E-3</v>
       </c>
       <c r="U33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>5.4945054945055027E-3</v>
       </c>
       <c r="V33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W33">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K34">
-        <f t="shared" ref="K34:P34" si="26">K10 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K10))</f>
+        <f t="shared" ref="K34:P34" si="30">K10 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K10))</f>
         <v>0.40322580645161288</v>
       </c>
       <c r="L34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0.32258064516129031</v>
       </c>
       <c r="M34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0.19354838709677419</v>
       </c>
       <c r="N34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>8.0645161290322578E-2</v>
       </c>
       <c r="O34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-5.9737156511350087E-2</v>
       </c>
       <c r="S34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4.4802867383512524E-2</v>
       </c>
       <c r="T34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>8.3632019115890133E-3</v>
       </c>
       <c r="U34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>6.5710872162485084E-3</v>
       </c>
       <c r="V34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K35">
-        <f t="shared" ref="K35:P35" si="27">K11 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K11))</f>
+        <f t="shared" ref="K35:P35" si="31">K11 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K11))</f>
         <v>0.38333333333333336</v>
       </c>
       <c r="L35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="M35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0.15</v>
       </c>
       <c r="N35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="O35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="R35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-5.8974358974358931E-2</v>
       </c>
       <c r="S35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4.0384615384615352E-2</v>
       </c>
       <c r="T35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>5.7692307692307765E-3</v>
       </c>
       <c r="U35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.2820512820512803E-2</v>
       </c>
       <c r="V35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W35">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -2454,97 +2457,97 @@
         <v>0.35714285714285715</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36:P36" si="28">L12 * L$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K12))</f>
+        <f t="shared" ref="L36:P36" si="32">L12 * L$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K12))</f>
         <v>0.25</v>
       </c>
       <c r="M36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="N36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.17857142857142858</v>
       </c>
       <c r="O36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-5.5228276877761384E-2</v>
       </c>
       <c r="S36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3.350515463917525E-2</v>
       </c>
       <c r="T36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>8.1001472754050063E-3</v>
       </c>
       <c r="U36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.3622974963181156E-2</v>
       </c>
       <c r="V36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K37">
-        <f t="shared" ref="K37:P37" si="29">K13 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K13))</f>
+        <f t="shared" ref="K37:P37" si="33">K13 * K$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K13))</f>
         <v>0.37037037037037035</v>
       </c>
       <c r="L37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="M37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="N37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>9.2592592592592587E-2</v>
       </c>
       <c r="O37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="P37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="R37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-5.5161544523246675E-2</v>
       </c>
       <c r="S37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3.0732860520094551E-2</v>
       </c>
       <c r="T37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>7.0921985815602662E-3</v>
       </c>
       <c r="U37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>7.4862096138691853E-3</v>
       </c>
       <c r="V37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>9.8502758077226027E-3</v>
       </c>
       <c r="W37">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -2554,47 +2557,47 @@
         <v>0.46</v>
       </c>
       <c r="L38">
-        <f t="shared" ref="K38:P38" si="30">L14 * L$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K14))</f>
+        <f t="shared" ref="L38:P38" si="34">L14 * L$16 / SUMPRODUCT($K$16:$P$16,_xlfn.ANCHORARRAY( $K14))</f>
         <v>0.32</v>
       </c>
       <c r="M38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0.12</v>
       </c>
       <c r="N38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0.1</v>
       </c>
       <c r="O38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="R38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-6.2727272727272687E-2</v>
       </c>
       <c r="S38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4.72727272727273E-2</v>
       </c>
       <c r="T38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>6.363636363636363E-3</v>
       </c>
       <c r="U38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>9.0909090909090939E-3</v>
       </c>
       <c r="V38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -2604,23 +2607,23 @@
         <v>0.28915662650602408</v>
       </c>
       <c r="L40">
-        <f t="shared" ref="L40:P40" si="31">L2 * L$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K2), $K$21:$P$21)</f>
+        <f t="shared" ref="L40:P40" si="35">L2 * L$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K2), $K$21:$P$21)</f>
         <v>0.19879518072289157</v>
       </c>
       <c r="M40">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0.21084337349397592</v>
       </c>
       <c r="N40">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>9.6385542168674704E-2</v>
       </c>
       <c r="O40">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>7.8313253012048195E-2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0.12650602409638553</v>
       </c>
       <c r="R40" s="2">
@@ -2628,19 +2631,19 @@
         <v>-5.4865400641962707E-2</v>
       </c>
       <c r="S40" s="2">
-        <f t="shared" ref="S40:W40" si="32">AVERAGE(S26:S38)</f>
+        <f t="shared" ref="S40:V40" si="36">AVERAGE(S26:S38)</f>
         <v>3.5992797136096405E-2</v>
       </c>
       <c r="T40" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6.6616254272271434E-3</v>
       </c>
       <c r="U40" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9.4094479921611306E-3</v>
       </c>
       <c r="V40" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>2.3286810766238453E-3</v>
       </c>
       <c r="W40" s="2">
@@ -2650,53 +2653,53 @@
     </row>
     <row r="41" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K41">
-        <f t="shared" ref="K41:P41" si="33">K3 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K3), $K$21:$P$21)</f>
+        <f t="shared" ref="K41:P41" si="37">K3 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K3), $K$21:$P$21)</f>
         <v>0.3546099290780142</v>
       </c>
       <c r="L41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.1702127659574468</v>
       </c>
       <c r="M41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.21276595744680851</v>
       </c>
       <c r="N41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.1702127659574468</v>
       </c>
       <c r="O41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>9.2198581560283682E-2</v>
       </c>
       <c r="P41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K42">
-        <f t="shared" ref="K42:P42" si="34">K4 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K4), $K$21:$P$21)</f>
+        <f t="shared" ref="K42:P42" si="38">K4 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K4), $K$21:$P$21)</f>
         <v>0.40601503759398494</v>
       </c>
       <c r="L42">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.22556390977443608</v>
       </c>
       <c r="M42">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.15037593984962405</v>
       </c>
       <c r="N42">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.12030075187969924</v>
       </c>
       <c r="O42">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>9.7744360902255634E-2</v>
       </c>
       <c r="P42">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R42" s="2">
@@ -2720,27 +2723,27 @@
     </row>
     <row r="43" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K43">
-        <f t="shared" ref="K43:P43" si="35">K5 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K5), $K$21:$P$21)</f>
+        <f t="shared" ref="K43:P43" si="39">K5 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K5), $K$21:$P$21)</f>
         <v>0.34586466165413532</v>
       </c>
       <c r="L43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0.24812030075187969</v>
       </c>
       <c r="M43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0.22556390977443608</v>
       </c>
       <c r="N43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0.18045112781954886</v>
       </c>
       <c r="O43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="P43">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="R43" s="2">
@@ -2764,53 +2767,53 @@
     </row>
     <row r="44" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K44">
-        <f t="shared" ref="K44:P44" si="36">K6 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K6), $K$21:$P$21)</f>
+        <f t="shared" ref="K44:P44" si="40">K6 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K6), $K$21:$P$21)</f>
         <v>0.35199999999999998</v>
       </c>
       <c r="L44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0.216</v>
       </c>
       <c r="M44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0.2</v>
       </c>
       <c r="N44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0.128</v>
       </c>
       <c r="O44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0.104</v>
       </c>
       <c r="P44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K45">
-        <f t="shared" ref="K45:P45" si="37">K7 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K7), $K$21:$P$21)</f>
+        <f t="shared" ref="K45:P45" si="41">K7 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K7), $K$21:$P$21)</f>
         <v>0.39669421487603307</v>
       </c>
       <c r="L45">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0.24793388429752067</v>
       </c>
       <c r="M45">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0.28925619834710742</v>
       </c>
       <c r="N45">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>6.6115702479338845E-2</v>
       </c>
       <c r="O45">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="P45">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="R45" t="s">
@@ -2819,27 +2822,27 @@
     </row>
     <row r="46" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K46">
-        <f t="shared" ref="K46:P46" si="38">K8 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K8), $K$21:$P$21)</f>
+        <f t="shared" ref="K46:P46" si="42">K8 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K8), $K$21:$P$21)</f>
         <v>0.46296296296296297</v>
       </c>
       <c r="L46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0.25</v>
       </c>
       <c r="M46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0.1388888888888889</v>
       </c>
       <c r="N46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="O46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P46">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="R46">
@@ -2857,37 +2860,37 @@
         <v>80</v>
       </c>
       <c r="V46">
-        <f t="shared" ref="V46" si="39">T46 + U46</f>
+        <f t="shared" ref="V46" si="43">T46 + U46</f>
         <v>130</v>
       </c>
       <c r="W46">
-        <f t="shared" ref="W46" si="40">U46 + V46</f>
+        <f t="shared" ref="W46" si="44">U46 + V46</f>
         <v>210</v>
       </c>
     </row>
     <row r="47" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K47">
-        <f t="shared" ref="K47:P47" si="41">K9 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K9), $K$21:$P$21)</f>
+        <f t="shared" ref="K47:P47" si="45">K9 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K9), $K$21:$P$21)</f>
         <v>0.4107142857142857</v>
       </c>
       <c r="L47">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.29464285714285715</v>
       </c>
       <c r="M47">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.22321428571428573</v>
       </c>
       <c r="N47">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="O47">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="P47">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="R47" t="s">
@@ -2896,131 +2899,131 @@
     </row>
     <row r="48" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K48">
-        <f t="shared" ref="K48:P48" si="42">K10 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K10), $K$21:$P$21)</f>
+        <f t="shared" ref="K48:P48" si="46">K10 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K10), $K$21:$P$21)</f>
         <v>0.46296296296296297</v>
       </c>
       <c r="L48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="M48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="N48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="O48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P48">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K49">
-        <f t="shared" ref="K49:P49" si="43">K11 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K11), $K$21:$P$21)</f>
+        <f t="shared" ref="K49:P49" si="47">K11 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K11), $K$21:$P$21)</f>
         <v>0.44230769230769229</v>
       </c>
       <c r="L49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.25961538461538464</v>
       </c>
       <c r="M49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.14423076923076922</v>
       </c>
       <c r="N49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="O49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K50">
-        <f t="shared" ref="K50:P50" si="44">K12 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K12), $K$21:$P$21)</f>
+        <f t="shared" ref="K50:P50" si="48">K12 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K12), $K$21:$P$21)</f>
         <v>0.41237113402061853</v>
       </c>
       <c r="L50">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0.21649484536082475</v>
       </c>
       <c r="M50">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0.20618556701030927</v>
       </c>
       <c r="N50">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0.16494845360824742</v>
       </c>
       <c r="O50">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K51">
-        <f t="shared" ref="K51:P51" si="45">K13 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K13), $K$21:$P$21)</f>
+        <f t="shared" ref="K51:P51" si="49">K13 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K13), $K$21:$P$21)</f>
         <v>0.42553191489361702</v>
       </c>
       <c r="L51">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0.19148936170212766</v>
       </c>
       <c r="M51">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0.15957446808510639</v>
       </c>
       <c r="N51">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>8.5106382978723402E-2</v>
       </c>
       <c r="O51">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0.13829787234042554</v>
       </c>
       <c r="P51">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K52">
-        <f t="shared" ref="K52:P52" si="46">K14 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K14), $K$21:$P$21)</f>
+        <f t="shared" ref="K52:P52" si="50">K14 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K14), $K$21:$P$21)</f>
         <v>0.52272727272727271</v>
       </c>
       <c r="L52">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="M52">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0.11363636363636363</v>
       </c>
       <c r="N52">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O52">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="P52">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dramatically simplified the first implementation
</commit_message>
<xml_diff>
--- a/static/marchMadness/marchMadnessTesting.xlsx
+++ b/static/marchMadness/marchMadnessTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/marchMadness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9D9301-36EA-4781-9417-AEA7BA861B59}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3518380-B3D4-43DA-A6F4-100F3A6E22BD}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{59FA6CC9-D02C-444C-8C9B-7D565C1F61C8}"/>
   </bookViews>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909BC3E6-1313-4909-83D8-6D1A2BDCBA9C}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -687,15 +687,15 @@
       </c>
       <c r="V2">
         <f t="shared" ref="V2:V14" si="1">SUMPRODUCT(_xlfn.ANCHORARRAY(K2), $K$21:$P$21)</f>
-        <v>1660</v>
+        <v>1715</v>
       </c>
       <c r="W2" s="2">
         <f>V2 / SUM($V$2:$V$14)</f>
-        <v>0.10849673202614379</v>
+        <v>0.10789556464296948</v>
       </c>
       <c r="X2">
         <f>V2 + 2*D2 + G2 * 25</f>
-        <v>1711</v>
+        <v>1766</v>
       </c>
       <c r="Y2">
         <f>_xlfn.RANK.AVG(X2, $X$2:$X$14)</f>
@@ -707,7 +707,7 @@
       </c>
       <c r="AB2">
         <f>AA2 / SUM($V$2:$V$14)</f>
-        <v>5.6209150326797387E-2</v>
+        <v>5.4105064485687325E-2</v>
       </c>
       <c r="AC2">
         <f>AA2 + D2 + G2 * 10</f>
@@ -773,15 +773,15 @@
       </c>
       <c r="V3">
         <f t="shared" si="1"/>
-        <v>1410</v>
+        <v>1450</v>
       </c>
       <c r="W3" s="2">
         <f>V3 / SUM($V$2:$V$14)</f>
-        <v>9.2156862745098045E-2</v>
+        <v>9.1223655237496065E-2</v>
       </c>
       <c r="X3">
         <f t="shared" ref="X3:X14" si="4">V3 + 2*D3 + G3 * 25</f>
-        <v>1475</v>
+        <v>1515</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y14" si="5">_xlfn.RANK.AVG(X3, $X$2:$X$14)</f>
@@ -793,7 +793,7 @@
       </c>
       <c r="AB3">
         <f t="shared" ref="AB3:AB14" si="7">AA3 / SUM($V$2:$V$14)</f>
-        <v>4.9673202614379082E-2</v>
+        <v>4.7813777917584149E-2</v>
       </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AC14" si="8">AA3 + D3 + G3 * 10</f>
@@ -859,15 +859,15 @@
       </c>
       <c r="V4">
         <f t="shared" si="1"/>
-        <v>1330</v>
+        <v>1380</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" ref="W4:W14" si="10">V4 / SUM($V$2:$V$14)</f>
-        <v>8.6928104575163395E-2</v>
+        <v>8.6819754639823846E-2</v>
       </c>
       <c r="X4">
         <f t="shared" si="4"/>
-        <v>1407</v>
+        <v>1457</v>
       </c>
       <c r="Y4">
         <f t="shared" si="5"/>
@@ -879,7 +879,7 @@
       </c>
       <c r="AB4">
         <f t="shared" si="7"/>
-        <v>4.7058823529411764E-2</v>
+        <v>4.5297263290342872E-2</v>
       </c>
       <c r="AC4">
         <f t="shared" si="8"/>
@@ -945,15 +945,15 @@
       </c>
       <c r="V5">
         <f t="shared" si="1"/>
-        <v>1330</v>
+        <v>1385</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="10"/>
-        <v>8.6928104575163395E-2</v>
+        <v>8.7134318968228999E-2</v>
       </c>
       <c r="X5">
         <f t="shared" si="4"/>
-        <v>1374</v>
+        <v>1429</v>
       </c>
       <c r="Y5">
         <f t="shared" si="5"/>
@@ -965,7 +965,7 @@
       </c>
       <c r="AB5">
         <f t="shared" si="7"/>
-        <v>4.9019607843137254E-2</v>
+        <v>4.7184649260773828E-2</v>
       </c>
       <c r="AC5">
         <f t="shared" si="8"/>
@@ -1031,15 +1031,15 @@
       </c>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>1250</v>
+        <v>1295</v>
       </c>
       <c r="W6" s="2">
         <f t="shared" si="10"/>
-        <v>8.1699346405228759E-2</v>
+        <v>8.1472161056936138E-2</v>
       </c>
       <c r="X6">
         <f t="shared" si="4"/>
-        <v>1312</v>
+        <v>1357</v>
       </c>
       <c r="Y6">
         <f t="shared" si="5"/>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="AB6">
         <f t="shared" si="7"/>
-        <v>4.4444444444444446E-2</v>
+        <v>4.2780748663101602E-2</v>
       </c>
       <c r="AC6">
         <f t="shared" si="8"/>
@@ -1117,15 +1117,15 @@
       </c>
       <c r="V7">
         <f t="shared" si="1"/>
-        <v>1210</v>
+        <v>1260</v>
       </c>
       <c r="W7" s="2">
         <f t="shared" si="10"/>
-        <v>7.9084967320261434E-2</v>
+        <v>7.9270210758100035E-2</v>
       </c>
       <c r="X7">
         <f t="shared" si="4"/>
-        <v>1277</v>
+        <v>1327</v>
       </c>
       <c r="Y7">
         <f t="shared" si="5"/>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="AB7">
         <f t="shared" si="7"/>
-        <v>4.5098039215686274E-2</v>
+        <v>4.3409877319911923E-2</v>
       </c>
       <c r="AC7">
         <f t="shared" si="8"/>
@@ -1203,15 +1203,15 @@
       </c>
       <c r="V8">
         <f t="shared" si="1"/>
-        <v>1080</v>
+        <v>1125</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="10"/>
-        <v>7.0588235294117646E-2</v>
+        <v>7.0776973891160735E-2</v>
       </c>
       <c r="X8">
         <f t="shared" si="4"/>
-        <v>1201</v>
+        <v>1246</v>
       </c>
       <c r="Y8">
         <f t="shared" si="5"/>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="AB8">
         <f t="shared" si="7"/>
-        <v>3.9215686274509803E-2</v>
+        <v>3.7747719408619061E-2</v>
       </c>
       <c r="AC8">
         <f t="shared" si="8"/>
@@ -1289,15 +1289,15 @@
       </c>
       <c r="V9">
         <f t="shared" si="1"/>
-        <v>1120</v>
+        <v>1175</v>
       </c>
       <c r="W9" s="2">
         <f t="shared" si="10"/>
-        <v>7.3202614379084971E-2</v>
+        <v>7.3922617175212327E-2</v>
       </c>
       <c r="X9">
         <f t="shared" si="4"/>
-        <v>1154</v>
+        <v>1209</v>
       </c>
       <c r="Y9">
         <f t="shared" si="5"/>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="AB9">
         <f t="shared" si="7"/>
-        <v>4.1830065359477121E-2</v>
+        <v>4.0264234035860332E-2</v>
       </c>
       <c r="AC9">
         <f t="shared" si="8"/>
@@ -1375,15 +1375,15 @@
       </c>
       <c r="V10">
         <f t="shared" si="1"/>
-        <v>1080</v>
+        <v>1130</v>
       </c>
       <c r="W10" s="2">
         <f t="shared" si="10"/>
-        <v>7.0588235294117646E-2</v>
+        <v>7.1091538219565903E-2</v>
       </c>
       <c r="X10">
         <f t="shared" si="4"/>
-        <v>1194</v>
+        <v>1244</v>
       </c>
       <c r="Y10">
         <f t="shared" si="5"/>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="AB10">
         <f t="shared" si="7"/>
-        <v>3.9869281045751631E-2</v>
+        <v>3.8376848065429382E-2</v>
       </c>
       <c r="AC10">
         <f t="shared" si="8"/>
@@ -1461,15 +1461,15 @@
       </c>
       <c r="V11">
         <f t="shared" si="1"/>
-        <v>1040</v>
+        <v>1085</v>
       </c>
       <c r="W11" s="2">
         <f t="shared" si="10"/>
-        <v>6.7973856209150321E-2</v>
+        <v>6.8260459263919465E-2</v>
       </c>
       <c r="X11">
         <f t="shared" si="4"/>
-        <v>1083</v>
+        <v>1128</v>
       </c>
       <c r="Y11">
         <f t="shared" si="5"/>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="AB11">
         <f t="shared" si="7"/>
-        <v>3.7908496732026141E-2</v>
+        <v>3.6489462094998426E-2</v>
       </c>
       <c r="AC11">
         <f t="shared" si="8"/>
@@ -1547,15 +1547,15 @@
       </c>
       <c r="V12">
         <f t="shared" si="1"/>
-        <v>970</v>
+        <v>1005</v>
       </c>
       <c r="W12" s="2">
         <f t="shared" si="10"/>
-        <v>6.3398692810457513E-2</v>
+        <v>6.3227430009436925E-2</v>
       </c>
       <c r="X12">
         <f t="shared" si="4"/>
-        <v>1019</v>
+        <v>1054</v>
       </c>
       <c r="Y12">
         <f t="shared" si="5"/>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="AB12">
         <f t="shared" si="7"/>
-        <v>3.5294117647058823E-2</v>
+        <v>3.3972947467757156E-2</v>
       </c>
       <c r="AC12">
         <f t="shared" si="8"/>
@@ -1633,15 +1633,15 @@
       </c>
       <c r="V13">
         <f t="shared" si="1"/>
-        <v>940</v>
+        <v>970</v>
       </c>
       <c r="W13" s="2">
         <f t="shared" si="10"/>
-        <v>6.1437908496732023E-2</v>
+        <v>6.1025479710600815E-2</v>
       </c>
       <c r="X13">
         <f t="shared" si="4"/>
-        <v>1031</v>
+        <v>1061</v>
       </c>
       <c r="Y13">
         <f t="shared" si="5"/>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="AB13">
         <f t="shared" si="7"/>
-        <v>3.2679738562091505E-2</v>
+        <v>3.1456432840515886E-2</v>
       </c>
       <c r="AC13">
         <f t="shared" si="8"/>
@@ -1719,15 +1719,15 @@
       </c>
       <c r="V14">
         <f t="shared" si="1"/>
-        <v>880</v>
+        <v>920</v>
       </c>
       <c r="W14" s="2">
         <f t="shared" si="10"/>
-        <v>5.7516339869281043E-2</v>
+        <v>5.787983642654923E-2</v>
       </c>
       <c r="X14">
         <f t="shared" si="4"/>
-        <v>964</v>
+        <v>1004</v>
       </c>
       <c r="Y14">
         <f t="shared" si="5"/>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="AB14">
         <f t="shared" si="7"/>
-        <v>3.202614379084967E-2</v>
+        <v>3.0827304183705568E-2</v>
       </c>
       <c r="AC14">
         <f t="shared" si="8"/>
@@ -1866,14 +1866,14 @@
         <v>20</v>
       </c>
       <c r="L21">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M21">
-        <f>K21 + L21</f>
+        <f>K21 + L21 - 5</f>
         <v>50</v>
       </c>
       <c r="N21">
-        <f>L21 + M21</f>
+        <f>L21 + M21 - 5</f>
         <v>80</v>
       </c>
       <c r="O21">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="14"/>
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
@@ -1918,19 +1918,19 @@
       </c>
       <c r="M23">
         <f>M21 / $L$21</f>
-        <v>1.6666666666666667</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="N23">
         <f>N21 / $L$21</f>
-        <v>2.6666666666666665</v>
+        <v>2.2857142857142856</v>
       </c>
       <c r="O23">
         <f>O21 / $L$21</f>
-        <v>4.333333333333333</v>
+        <v>3.7142857142857144</v>
       </c>
       <c r="P23">
         <f>P21 / $L$21</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="11:23" x14ac:dyDescent="0.55000000000000004">
@@ -1978,27 +1978,27 @@
       </c>
       <c r="R26">
         <f>K26 - K40</f>
-        <v>-4.425866732235062E-2</v>
+        <v>-3.4985422740524796E-2</v>
       </c>
       <c r="S26">
         <f>L26 - L40</f>
-        <v>2.5694615195475778E-2</v>
+        <v>0</v>
       </c>
       <c r="T26">
         <f t="shared" ref="T26:W26" si="16">M26 - M40</f>
-        <v>3.4423407917383575E-3</v>
+        <v>1.0204081632653045E-2</v>
       </c>
       <c r="U26">
         <f t="shared" si="16"/>
-        <v>5.6552741578559107E-3</v>
+        <v>8.7463556851311991E-3</v>
       </c>
       <c r="V26">
         <f t="shared" si="16"/>
-        <v>3.3194000491762882E-3</v>
+        <v>5.8309037900874522E-3</v>
       </c>
       <c r="W26">
         <f t="shared" si="16"/>
-        <v>6.1470371281042713E-3</v>
+        <v>1.0204081632653073E-2</v>
       </c>
     </row>
     <row r="27" spans="11:23" x14ac:dyDescent="0.55000000000000004">
@@ -2028,23 +2028,23 @@
       </c>
       <c r="R27">
         <f t="shared" ref="R27:R38" si="18">K27 - K41</f>
-        <v>-4.9731880297526398E-2</v>
+        <v>-3.9949537426408777E-2</v>
       </c>
       <c r="S27">
         <f t="shared" ref="S27:S38" si="19">L27 - L41</f>
-        <v>2.4909185262065398E-2</v>
+        <v>2.0185029436501356E-3</v>
       </c>
       <c r="T27">
         <f t="shared" ref="T27:T38" si="20">M27 - M41</f>
-        <v>6.7462376751427078E-3</v>
+        <v>1.2615643397813292E-2</v>
       </c>
       <c r="U27">
         <f t="shared" ref="U27:U38" si="21">N27 - N41</f>
-        <v>1.2714063310845874E-2</v>
+        <v>1.7409587888982336E-2</v>
       </c>
       <c r="V27">
         <f t="shared" ref="V27:V38" si="22">O27 - O41</f>
-        <v>5.3623940494724187E-3</v>
+        <v>7.9058031959629987E-3</v>
       </c>
       <c r="W27">
         <f t="shared" ref="W27:W38" si="23">P27 - P41</f>
@@ -2078,23 +2078,23 @@
       </c>
       <c r="R28">
         <f t="shared" si="18"/>
-        <v>-5.5365686944634285E-2</v>
+        <v>-4.0654997176736318E-2</v>
       </c>
       <c r="S28">
         <f t="shared" si="19"/>
-        <v>3.4176349965823638E-2</v>
+        <v>6.1170713344625982E-3</v>
       </c>
       <c r="T28">
         <f t="shared" si="20"/>
-        <v>5.4682159945317887E-3</v>
+        <v>1.0916619612271777E-2</v>
       </c>
       <c r="U28">
         <f t="shared" si="21"/>
-        <v>9.5693779904306164E-3</v>
+        <v>1.392810088462261E-2</v>
       </c>
       <c r="V28">
         <f t="shared" si="22"/>
-        <v>6.1517429938482693E-3</v>
+        <v>9.6932053453792633E-3</v>
       </c>
       <c r="W28">
         <f t="shared" si="23"/>
@@ -2128,19 +2128,19 @@
       </c>
       <c r="R29">
         <f t="shared" si="18"/>
-        <v>-5.099286678234044E-2</v>
+        <v>-3.725816902712209E-2</v>
       </c>
       <c r="S29">
         <f t="shared" si="19"/>
-        <v>3.3930981299402363E-2</v>
+        <v>4.072942701101534E-3</v>
       </c>
       <c r="T29">
         <f t="shared" si="20"/>
-        <v>5.2053209947947043E-3</v>
+        <v>1.4162732574284936E-2</v>
       </c>
       <c r="U29">
         <f t="shared" si="21"/>
-        <v>1.1856564488143456E-2</v>
+        <v>1.9022493751735647E-2</v>
       </c>
       <c r="V29">
         <f t="shared" si="22"/>
@@ -2178,23 +2178,23 @@
       </c>
       <c r="R30">
         <f t="shared" si="18"/>
-        <v>-5.0630136986301366E-2</v>
+        <v>-3.8398476754641142E-2</v>
       </c>
       <c r="S30">
         <f t="shared" si="19"/>
-        <v>3.0575342465753413E-2</v>
+        <v>3.3320992225101542E-3</v>
       </c>
       <c r="T30">
         <f t="shared" si="20"/>
-        <v>5.479452054794498E-3</v>
+        <v>1.2429259004601456E-2</v>
       </c>
       <c r="U30">
         <f t="shared" si="21"/>
-        <v>8.9863013698630034E-3</v>
+        <v>1.3434177817739451E-2</v>
       </c>
       <c r="V30">
         <f t="shared" si="22"/>
-        <v>5.5890410958904096E-3</v>
+        <v>9.2029407097900251E-3</v>
       </c>
       <c r="W30">
         <f t="shared" si="23"/>
@@ -2228,19 +2228,19 @@
       </c>
       <c r="R31">
         <f t="shared" si="18"/>
-        <v>-5.3837072018890209E-2</v>
+        <v>-3.8095238095238071E-2</v>
       </c>
       <c r="S31">
         <f t="shared" si="19"/>
-        <v>3.778040141676503E-2</v>
+        <v>7.9365079365079083E-3</v>
       </c>
       <c r="T31">
         <f t="shared" si="20"/>
-        <v>1.0743801652892571E-2</v>
+        <v>2.2222222222222199E-2</v>
       </c>
       <c r="U31">
         <f t="shared" si="21"/>
-        <v>5.3128689492325798E-3</v>
+        <v>7.9365079365079361E-3</v>
       </c>
       <c r="V31">
         <f t="shared" si="22"/>
@@ -2278,19 +2278,19 @@
       </c>
       <c r="R32">
         <f t="shared" si="18"/>
-        <v>-5.9737156511350087E-2</v>
+        <v>-4.1218637992831542E-2</v>
       </c>
       <c r="S32">
         <f t="shared" si="19"/>
-        <v>4.032258064516131E-2</v>
+        <v>1.0322580645161283E-2</v>
       </c>
       <c r="T32">
         <f t="shared" si="20"/>
-        <v>6.27240143369176E-3</v>
+        <v>1.1827956989247324E-2</v>
       </c>
       <c r="U32">
         <f t="shared" si="21"/>
-        <v>1.3142174432497017E-2</v>
+        <v>1.9068100358422935E-2</v>
       </c>
       <c r="V32">
         <f t="shared" si="22"/>
@@ -2328,19 +2328,19 @@
       </c>
       <c r="R33">
         <f t="shared" si="18"/>
-        <v>-5.6868131868131833E-2</v>
+        <v>-3.7643207855973804E-2</v>
       </c>
       <c r="S33">
         <f t="shared" si="19"/>
-        <v>4.381868131868133E-2</v>
+        <v>1.0801963993453401E-2</v>
       </c>
       <c r="T33">
         <f t="shared" si="20"/>
-        <v>7.5549450549450559E-3</v>
+        <v>1.800327332242227E-2</v>
       </c>
       <c r="U33">
         <f t="shared" si="21"/>
-        <v>5.4945054945055027E-3</v>
+        <v>8.8379705400982028E-3</v>
       </c>
       <c r="V33">
         <f t="shared" si="22"/>
@@ -2378,19 +2378,19 @@
       </c>
       <c r="R34">
         <f t="shared" si="18"/>
-        <v>-5.9737156511350087E-2</v>
+        <v>-3.9252069654581834E-2</v>
       </c>
       <c r="S34">
         <f t="shared" si="19"/>
-        <v>4.4802867383512524E-2</v>
+        <v>1.2846131886954049E-2</v>
       </c>
       <c r="T34">
         <f t="shared" si="20"/>
-        <v>8.3632019115890133E-3</v>
+        <v>1.6557236654296315E-2</v>
       </c>
       <c r="U34">
         <f t="shared" si="21"/>
-        <v>6.5710872162485084E-3</v>
+        <v>9.8487011133314289E-3</v>
       </c>
       <c r="V34">
         <f t="shared" si="22"/>
@@ -2428,19 +2428,19 @@
       </c>
       <c r="R35">
         <f t="shared" si="18"/>
-        <v>-5.8974358974358931E-2</v>
+        <v>-4.0629800307219632E-2</v>
       </c>
       <c r="S35">
         <f t="shared" si="19"/>
-        <v>4.0384615384615352E-2</v>
+        <v>9.6774193548386789E-3</v>
       </c>
       <c r="T35">
         <f t="shared" si="20"/>
-        <v>5.7692307692307765E-3</v>
+        <v>1.1751152073732701E-2</v>
       </c>
       <c r="U35">
         <f t="shared" si="21"/>
-        <v>1.2820512820512803E-2</v>
+        <v>1.9201228878648224E-2</v>
       </c>
       <c r="V35">
         <f t="shared" si="22"/>
@@ -2478,19 +2478,19 @@
       </c>
       <c r="R36">
         <f t="shared" si="18"/>
-        <v>-5.5228276877761384E-2</v>
+        <v>-4.0867093105899088E-2</v>
       </c>
       <c r="S36">
         <f t="shared" si="19"/>
-        <v>3.350515463917525E-2</v>
+        <v>6.2189054726368154E-3</v>
       </c>
       <c r="T36">
         <f t="shared" si="20"/>
-        <v>8.1001472754050063E-3</v>
+        <v>1.5280739161336154E-2</v>
       </c>
       <c r="U36">
         <f t="shared" si="21"/>
-        <v>1.3622974963181156E-2</v>
+        <v>1.9367448471926091E-2</v>
       </c>
       <c r="V36">
         <f t="shared" si="22"/>
@@ -2528,23 +2528,23 @@
       </c>
       <c r="R37">
         <f t="shared" si="18"/>
-        <v>-5.5161544523246675E-2</v>
+        <v>-4.2000763650248185E-2</v>
       </c>
       <c r="S37">
         <f t="shared" si="19"/>
-        <v>3.0732860520094551E-2</v>
+        <v>5.7273768613974596E-3</v>
       </c>
       <c r="T37">
         <f t="shared" si="20"/>
-        <v>7.0921985815602662E-3</v>
+        <v>1.2027491408934693E-2</v>
       </c>
       <c r="U37">
         <f t="shared" si="21"/>
-        <v>7.4862096138691853E-3</v>
+        <v>1.0118365788468878E-2</v>
       </c>
       <c r="V37">
         <f t="shared" si="22"/>
-        <v>9.8502758077226027E-3</v>
+        <v>1.4127529591447113E-2</v>
       </c>
       <c r="W37">
         <f t="shared" si="23"/>
@@ -2578,19 +2578,19 @@
       </c>
       <c r="R38">
         <f t="shared" si="18"/>
-        <v>-6.2727272727272687E-2</v>
+        <v>-3.999999999999998E-2</v>
       </c>
       <c r="S38">
         <f t="shared" si="19"/>
-        <v>4.72727272727273E-2</v>
+        <v>1.5652173913043466E-2</v>
       </c>
       <c r="T38">
         <f t="shared" si="20"/>
-        <v>6.363636363636363E-3</v>
+        <v>1.1304347826086955E-2</v>
       </c>
       <c r="U38">
         <f t="shared" si="21"/>
-        <v>9.0909090909090939E-3</v>
+        <v>1.3043478260869573E-2</v>
       </c>
       <c r="V38">
         <f t="shared" si="22"/>
@@ -2604,73 +2604,73 @@
     <row r="40" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K40">
         <f>K2 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K2), $K$21:$P$21)</f>
-        <v>0.28915662650602408</v>
+        <v>0.27988338192419826</v>
       </c>
       <c r="L40">
         <f t="shared" ref="L40:P40" si="35">L2 * L$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K2), $K$21:$P$21)</f>
-        <v>0.19879518072289157</v>
+        <v>0.22448979591836735</v>
       </c>
       <c r="M40">
         <f t="shared" si="35"/>
-        <v>0.21084337349397592</v>
+        <v>0.20408163265306123</v>
       </c>
       <c r="N40">
         <f t="shared" si="35"/>
-        <v>9.6385542168674704E-2</v>
+        <v>9.3294460641399415E-2</v>
       </c>
       <c r="O40">
         <f t="shared" si="35"/>
-        <v>7.8313253012048195E-2</v>
+        <v>7.5801749271137031E-2</v>
       </c>
       <c r="P40">
         <f t="shared" si="35"/>
-        <v>0.12650602409638553</v>
+        <v>0.12244897959183673</v>
       </c>
       <c r="R40" s="2">
         <f>AVERAGE(R26:R38)</f>
-        <v>-5.4865400641962707E-2</v>
+        <v>-3.9304108752878861E-2</v>
       </c>
       <c r="S40" s="2">
         <f t="shared" ref="S40:V40" si="36">AVERAGE(S26:S38)</f>
-        <v>3.5992797136096405E-2</v>
+        <v>7.2864366358244221E-3</v>
       </c>
       <c r="T40" s="2">
         <f t="shared" si="36"/>
-        <v>6.6616254272271434E-3</v>
+        <v>1.3792519683069472E-2</v>
       </c>
       <c r="U40" s="2">
         <f t="shared" si="36"/>
-        <v>9.4094479921611306E-3</v>
+        <v>1.3843270567421887E-2</v>
       </c>
       <c r="V40" s="2">
         <f t="shared" si="36"/>
-        <v>2.3286810766238453E-3</v>
+        <v>3.5969525102051425E-3</v>
       </c>
       <c r="W40" s="2">
         <f>AVERAGE(W26:W38)</f>
-        <v>4.7284900985417473E-4</v>
+        <v>7.849293563579287E-4</v>
       </c>
     </row>
     <row r="41" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K41">
         <f t="shared" ref="K41:P41" si="37">K3 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K3), $K$21:$P$21)</f>
-        <v>0.3546099290780142</v>
+        <v>0.34482758620689657</v>
       </c>
       <c r="L41">
         <f t="shared" si="37"/>
-        <v>0.1702127659574468</v>
+        <v>0.19310344827586207</v>
       </c>
       <c r="M41">
         <f t="shared" si="37"/>
-        <v>0.21276595744680851</v>
+        <v>0.20689655172413793</v>
       </c>
       <c r="N41">
         <f t="shared" si="37"/>
-        <v>0.1702127659574468</v>
+        <v>0.16551724137931034</v>
       </c>
       <c r="O41">
         <f t="shared" si="37"/>
-        <v>9.2198581560283682E-2</v>
+        <v>8.9655172413793102E-2</v>
       </c>
       <c r="P41">
         <f t="shared" si="37"/>
@@ -2680,23 +2680,23 @@
     <row r="42" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K42">
         <f t="shared" ref="K42:P42" si="38">K4 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K4), $K$21:$P$21)</f>
-        <v>0.40601503759398494</v>
+        <v>0.39130434782608697</v>
       </c>
       <c r="L42">
         <f t="shared" si="38"/>
-        <v>0.22556390977443608</v>
+        <v>0.25362318840579712</v>
       </c>
       <c r="M42">
         <f t="shared" si="38"/>
-        <v>0.15037593984962405</v>
+        <v>0.14492753623188406</v>
       </c>
       <c r="N42">
         <f t="shared" si="38"/>
-        <v>0.12030075187969924</v>
+        <v>0.11594202898550725</v>
       </c>
       <c r="O42">
         <f t="shared" si="38"/>
-        <v>9.7744360902255634E-2</v>
+        <v>9.420289855072464E-2</v>
       </c>
       <c r="P42">
         <f t="shared" si="38"/>
@@ -2724,19 +2724,19 @@
     <row r="43" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K43">
         <f t="shared" ref="K43:P43" si="39">K5 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K5), $K$21:$P$21)</f>
-        <v>0.34586466165413532</v>
+        <v>0.33212996389891697</v>
       </c>
       <c r="L43">
         <f t="shared" si="39"/>
-        <v>0.24812030075187969</v>
+        <v>0.27797833935018051</v>
       </c>
       <c r="M43">
         <f t="shared" si="39"/>
-        <v>0.22556390977443608</v>
+        <v>0.21660649819494585</v>
       </c>
       <c r="N43">
         <f t="shared" si="39"/>
-        <v>0.18045112781954886</v>
+        <v>0.17328519855595667</v>
       </c>
       <c r="O43">
         <f t="shared" si="39"/>
@@ -2768,23 +2768,23 @@
     <row r="44" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K44">
         <f t="shared" ref="K44:P44" si="40">K6 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K6), $K$21:$P$21)</f>
-        <v>0.35199999999999998</v>
+        <v>0.33976833976833976</v>
       </c>
       <c r="L44">
         <f t="shared" si="40"/>
-        <v>0.216</v>
+        <v>0.24324324324324326</v>
       </c>
       <c r="M44">
         <f t="shared" si="40"/>
-        <v>0.2</v>
+        <v>0.19305019305019305</v>
       </c>
       <c r="N44">
         <f t="shared" si="40"/>
-        <v>0.128</v>
+        <v>0.12355212355212356</v>
       </c>
       <c r="O44">
         <f t="shared" si="40"/>
-        <v>0.104</v>
+        <v>0.10038610038610038</v>
       </c>
       <c r="P44">
         <f t="shared" si="40"/>
@@ -2794,19 +2794,19 @@
     <row r="45" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K45">
         <f t="shared" ref="K45:P45" si="41">K7 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K7), $K$21:$P$21)</f>
-        <v>0.39669421487603307</v>
+        <v>0.38095238095238093</v>
       </c>
       <c r="L45">
         <f t="shared" si="41"/>
-        <v>0.24793388429752067</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="M45">
         <f t="shared" si="41"/>
-        <v>0.28925619834710742</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="N45">
         <f t="shared" si="41"/>
-        <v>6.6115702479338845E-2</v>
+        <v>6.3492063492063489E-2</v>
       </c>
       <c r="O45">
         <f t="shared" si="41"/>
@@ -2823,19 +2823,19 @@
     <row r="46" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K46">
         <f t="shared" ref="K46:P46" si="42">K8 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K8), $K$21:$P$21)</f>
-        <v>0.46296296296296297</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L46">
         <f t="shared" si="42"/>
-        <v>0.25</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M46">
         <f t="shared" si="42"/>
-        <v>0.1388888888888889</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="N46">
         <f t="shared" si="42"/>
-        <v>0.14814814814814814</v>
+        <v>0.14222222222222222</v>
       </c>
       <c r="O46">
         <f t="shared" si="42"/>
@@ -2871,19 +2871,19 @@
     <row r="47" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K47">
         <f t="shared" ref="K47:P47" si="45">K9 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K9), $K$21:$P$21)</f>
-        <v>0.4107142857142857</v>
+        <v>0.39148936170212767</v>
       </c>
       <c r="L47">
         <f t="shared" si="45"/>
-        <v>0.29464285714285715</v>
+        <v>0.32765957446808508</v>
       </c>
       <c r="M47">
         <f t="shared" si="45"/>
-        <v>0.22321428571428573</v>
+        <v>0.21276595744680851</v>
       </c>
       <c r="N47">
         <f t="shared" si="45"/>
-        <v>7.1428571428571425E-2</v>
+        <v>6.8085106382978725E-2</v>
       </c>
       <c r="O47">
         <f t="shared" si="45"/>
@@ -2900,19 +2900,19 @@
     <row r="48" spans="11:23" x14ac:dyDescent="0.55000000000000004">
       <c r="K48">
         <f t="shared" ref="K48:P48" si="46">K10 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K10), $K$21:$P$21)</f>
-        <v>0.46296296296296297</v>
+        <v>0.44247787610619471</v>
       </c>
       <c r="L48">
         <f t="shared" si="46"/>
-        <v>0.27777777777777779</v>
+        <v>0.30973451327433627</v>
       </c>
       <c r="M48">
         <f t="shared" si="46"/>
-        <v>0.18518518518518517</v>
+        <v>0.17699115044247787</v>
       </c>
       <c r="N48">
         <f t="shared" si="46"/>
-        <v>7.407407407407407E-2</v>
+        <v>7.0796460176991149E-2</v>
       </c>
       <c r="O48">
         <f t="shared" si="46"/>
@@ -2926,19 +2926,19 @@
     <row r="49" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K49">
         <f t="shared" ref="K49:P49" si="47">K11 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K11), $K$21:$P$21)</f>
-        <v>0.44230769230769229</v>
+        <v>0.42396313364055299</v>
       </c>
       <c r="L49">
         <f t="shared" si="47"/>
-        <v>0.25961538461538464</v>
+        <v>0.29032258064516131</v>
       </c>
       <c r="M49">
         <f t="shared" si="47"/>
-        <v>0.14423076923076922</v>
+        <v>0.13824884792626729</v>
       </c>
       <c r="N49">
         <f t="shared" si="47"/>
-        <v>0.15384615384615385</v>
+        <v>0.14746543778801843</v>
       </c>
       <c r="O49">
         <f t="shared" si="47"/>
@@ -2952,19 +2952,19 @@
     <row r="50" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K50">
         <f t="shared" ref="K50:P50" si="48">K12 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K12), $K$21:$P$21)</f>
-        <v>0.41237113402061853</v>
+        <v>0.39800995024875624</v>
       </c>
       <c r="L50">
         <f t="shared" si="48"/>
-        <v>0.21649484536082475</v>
+        <v>0.24378109452736318</v>
       </c>
       <c r="M50">
         <f t="shared" si="48"/>
-        <v>0.20618556701030927</v>
+        <v>0.19900497512437812</v>
       </c>
       <c r="N50">
         <f t="shared" si="48"/>
-        <v>0.16494845360824742</v>
+        <v>0.15920398009950248</v>
       </c>
       <c r="O50">
         <f t="shared" si="48"/>
@@ -2978,23 +2978,23 @@
     <row r="51" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K51">
         <f t="shared" ref="K51:P51" si="49">K13 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K13), $K$21:$P$21)</f>
-        <v>0.42553191489361702</v>
+        <v>0.41237113402061853</v>
       </c>
       <c r="L51">
         <f t="shared" si="49"/>
-        <v>0.19148936170212766</v>
+        <v>0.21649484536082475</v>
       </c>
       <c r="M51">
         <f t="shared" si="49"/>
-        <v>0.15957446808510639</v>
+        <v>0.15463917525773196</v>
       </c>
       <c r="N51">
         <f t="shared" si="49"/>
-        <v>8.5106382978723402E-2</v>
+        <v>8.247422680412371E-2</v>
       </c>
       <c r="O51">
         <f t="shared" si="49"/>
-        <v>0.13829787234042554</v>
+        <v>0.13402061855670103</v>
       </c>
       <c r="P51">
         <f t="shared" si="49"/>
@@ -3004,19 +3004,19 @@
     <row r="52" spans="11:16" x14ac:dyDescent="0.55000000000000004">
       <c r="K52">
         <f t="shared" ref="K52:P52" si="50">K14 * K$21 / SUMPRODUCT(_xlfn.ANCHORARRAY($K14), $K$21:$P$21)</f>
-        <v>0.52272727272727271</v>
+        <v>0.5</v>
       </c>
       <c r="L52">
         <f t="shared" si="50"/>
-        <v>0.27272727272727271</v>
+        <v>0.30434782608695654</v>
       </c>
       <c r="M52">
         <f t="shared" si="50"/>
-        <v>0.11363636363636363</v>
+        <v>0.10869565217391304</v>
       </c>
       <c r="N52">
         <f t="shared" si="50"/>
-        <v>9.0909090909090912E-2</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="O52">
         <f t="shared" si="50"/>

</xml_diff>

<commit_message>
added most of the bonus star categories
</commit_message>
<xml_diff>
--- a/static/marchMadness/marchMadnessTesting.xlsx
+++ b/static/marchMadness/marchMadnessTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/marchMadness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3518380-B3D4-43DA-A6F4-100F3A6E22BD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08561CEF-5C63-4E24-9320-63416865CAA8}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{59FA6CC9-D02C-444C-8C9B-7D565C1F61C8}"/>
   </bookViews>
@@ -573,12 +573,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909BC3E6-1313-4909-83D8-6D1A2BDCBA9C}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="4" max="4" width="6.734375" customWidth="1"/>
     <col min="6" max="6" width="14.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated hightlight to bracket to make it more obvious which games are unplayed and next. also added hover feature to the standings page bracket
</commit_message>
<xml_diff>
--- a/static/marchMadness/marchMadnessTesting.xlsx
+++ b/static/marchMadness/marchMadnessTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/marchMadness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08561CEF-5C63-4E24-9320-63416865CAA8}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{66257C57-8D1C-42A7-A216-1A6E460CDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{145A1C1D-0412-45C0-9B4F-FB3981A0A416}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{59FA6CC9-D02C-444C-8C9B-7D565C1F61C8}"/>
   </bookViews>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909BC3E6-1313-4909-83D8-6D1A2BDCBA9C}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>